<commit_message>
Updating the changes of MapsAPI with cucumber framework
</commit_message>
<xml_diff>
--- a/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
+++ b/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="46">
   <si>
     <t>ProjectName</t>
   </si>
@@ -85,12 +85,6 @@
     <t>TestModule</t>
   </si>
   <si>
-    <t>TestcaseId</t>
-  </si>
-  <si>
-    <t>TestClass</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -112,39 +106,9 @@
     <t>Resources//config.properties</t>
   </si>
   <si>
-    <t>RestAPI-Testing-Jira</t>
-  </si>
-  <si>
     <t>Resource</t>
   </si>
   <si>
-    <t>fasiddiqh72@gmail.com</t>
-  </si>
-  <si>
-    <t>getAuthCode</t>
-  </si>
-  <si>
-    <t>AuthUrl</t>
-  </si>
-  <si>
-    <t>https://accounts.google.com/o/oauth2/v2/auth?scope=https://www.googleapis.com/auth/userinfo.email&amp;auth_url=https://accounts.google.com/o/oauth2/v2/auth&amp;client_id=692183103107-p0m7ent2hk7suguv4vq22hjcfhcr43pj.apps.googleusercontent.com&amp;response_type=code&amp;redirect_uri=https://rahulshettyacademy.com/getCourse.php&amp;status=sdadadada</t>
-  </si>
-  <si>
-    <t>******</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>getAccessToken</t>
-  </si>
-  <si>
-    <t>692183103107-p0m7ent2hk7suguv4vq22hjcfhcr43pj.apps.googleusercontent.com</t>
-  </si>
-  <si>
-    <t>Client_Id</t>
-  </si>
-  <si>
     <t>Client_secret</t>
   </si>
   <si>
@@ -176,6 +140,33 @@
   </si>
   <si>
     <t>Maps</t>
+  </si>
+  <si>
+    <t>RestAPI-Testing-Maps</t>
+  </si>
+  <si>
+    <t>AddPlace</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>(+91) 983 893 3937</t>
+  </si>
+  <si>
+    <t>website</t>
+  </si>
+  <si>
+    <t>www.google.com</t>
+  </si>
+  <si>
+    <t>types</t>
+  </si>
+  <si>
+    <t>My Shop:Raymonds , The Stopper's Stop</t>
+  </si>
+  <si>
+    <t>accuracy</t>
   </si>
 </sst>
 </file>
@@ -601,14 +592,14 @@
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" t="e">
         <f>-C4</f>
         <v>#VALUE!</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -661,7 +652,7 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -675,7 +666,7 @@
         <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
         <v>14</v>
@@ -689,7 +680,7 @@
         <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
@@ -705,26 +696,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G84"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.109375" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="25.6640625" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" customWidth="1"/>
-    <col min="5" max="5" width="43.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" customWidth="1"/>
-    <col min="7" max="7" width="107.77734375" style="4" customWidth="1"/>
+    <col min="3" max="3" width="43.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="107.77734375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>17</v>
@@ -733,453 +722,332 @@
         <v>19</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="str">
+        <f>(C2)</f>
+        <v>AddPlace</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ref="C4:C9" si="0">(C3)</f>
+        <v>AddPlace</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>AddPlace</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>AddPlace</v>
+      </c>
+      <c r="D6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>AddPlace</v>
+      </c>
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="E2" t="s">
+      <c r="E7" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>AddPlace</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E8" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="9" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>AddPlace</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="E3" t="str">
-        <f>(E2)</f>
-        <v>getAuthCode</v>
-      </c>
-      <c r="F3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="E4" t="str">
-        <f t="shared" ref="E4:E9" si="0">(E3)</f>
-        <v>getAuthCode</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="E5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F5" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="E6" t="str">
-        <f t="shared" si="0"/>
-        <v>getAccessToken</v>
-      </c>
-      <c r="F6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="E7" t="str">
-        <f t="shared" si="0"/>
-        <v>getAccessToken</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="E8" t="str">
-        <f t="shared" si="0"/>
-        <v>getAccessToken</v>
-      </c>
-      <c r="F8" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v>getAccessToken</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="E10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="3"/>
-    </row>
-    <row r="16" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="3:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="3"/>
-    </row>
-    <row r="27" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="3"/>
-    </row>
-    <row r="28" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="3"/>
-    </row>
-    <row r="29" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="3"/>
-    </row>
-    <row r="31" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="3"/>
-    </row>
-    <row r="33" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="3"/>
-    </row>
-    <row r="34" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="3"/>
-    </row>
-    <row r="35" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="3"/>
-    </row>
-    <row r="36" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="3"/>
-    </row>
-    <row r="37" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="3"/>
-    </row>
-    <row r="38" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="3"/>
-    </row>
-    <row r="39" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="3"/>
-    </row>
-    <row r="40" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="3"/>
-    </row>
-    <row r="41" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="3"/>
-    </row>
-    <row r="42" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="3"/>
-    </row>
-    <row r="43" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C44" s="3"/>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C45" s="3"/>
-      <c r="E45" s="2"/>
-    </row>
-    <row r="46" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C46" s="3"/>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C47" s="3"/>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C48" s="3"/>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C49" s="3"/>
-      <c r="E49" s="2"/>
-    </row>
-    <row r="50" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C50" s="3"/>
-      <c r="E50" s="2"/>
-    </row>
-    <row r="51" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C51" s="3"/>
-      <c r="E51" s="2"/>
-    </row>
-    <row r="52" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C52" s="3"/>
-      <c r="E52" s="2"/>
-    </row>
-    <row r="53" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C53" s="3"/>
-      <c r="E53" s="2"/>
-    </row>
-    <row r="54" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C54" s="3"/>
-      <c r="E54" s="2"/>
-    </row>
-    <row r="55" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C55" s="3"/>
-      <c r="E55" s="2"/>
-    </row>
-    <row r="56" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C56" s="3"/>
-      <c r="E56" s="2"/>
-    </row>
-    <row r="57" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C57" s="3"/>
-      <c r="E57" s="2"/>
-    </row>
-    <row r="58" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C58" s="3"/>
-      <c r="E58" s="2"/>
-    </row>
-    <row r="59" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C59" s="3"/>
-      <c r="E59" s="2"/>
-    </row>
-    <row r="60" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C60" s="3"/>
-      <c r="E60" s="2"/>
-    </row>
-    <row r="61" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C61" s="3"/>
-      <c r="E61" s="2"/>
-    </row>
-    <row r="62" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C62" s="3"/>
-      <c r="E62" s="2"/>
-    </row>
-    <row r="63" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C63" s="3"/>
-      <c r="E63" s="2"/>
-    </row>
-    <row r="64" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C64" s="3"/>
-      <c r="E64" s="2"/>
-    </row>
-    <row r="65" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C65" s="3"/>
-      <c r="E65" s="2"/>
-    </row>
-    <row r="66" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C66" s="3"/>
-      <c r="E66" s="2"/>
-    </row>
-    <row r="67" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C67" s="3"/>
-      <c r="E67" s="2"/>
-    </row>
-    <row r="68" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C68" s="3"/>
-      <c r="E68" s="2"/>
-    </row>
-    <row r="69" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C69" s="3"/>
-      <c r="E69" s="2"/>
-    </row>
-    <row r="70" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C70" s="3"/>
-      <c r="E70" s="2"/>
-    </row>
-    <row r="71" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C71" s="3"/>
-      <c r="E71" s="2"/>
-    </row>
-    <row r="72" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C72" s="3"/>
-      <c r="E72" s="2"/>
-    </row>
-    <row r="73" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C73" s="3"/>
-      <c r="E73" s="2"/>
-    </row>
-    <row r="74" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C74" s="3"/>
-      <c r="E74" s="2"/>
-    </row>
-    <row r="75" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C75" s="3"/>
-      <c r="E75" s="2"/>
-    </row>
-    <row r="76" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C76" s="3"/>
-      <c r="E76" s="2"/>
-    </row>
-    <row r="77" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C77" s="3"/>
-      <c r="E77" s="2"/>
-    </row>
-    <row r="78" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C78" s="3"/>
-      <c r="E78" s="2"/>
-    </row>
-    <row r="79" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C79" s="3"/>
-      <c r="E79" s="2"/>
-    </row>
-    <row r="80" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C80" s="3"/>
-      <c r="E80" s="2"/>
-    </row>
-    <row r="81" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C81" s="3"/>
-      <c r="E81" s="2"/>
-    </row>
-    <row r="82" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C82" s="3"/>
-      <c r="E82" s="2"/>
-    </row>
-    <row r="83" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C83" s="3"/>
-      <c r="E83" s="2"/>
-    </row>
-    <row r="84" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C84" s="3"/>
-      <c r="E84" s="2"/>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="12" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="29" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="30" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="31" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="32" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="33" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="3:3" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C44" s="2"/>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C45" s="2"/>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C46" s="2"/>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C47" s="2"/>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C48" s="2"/>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C50" s="2"/>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C52" s="2"/>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C53" s="2"/>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C54" s="2"/>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C55" s="2"/>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C56" s="2"/>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C57" s="2"/>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C58" s="2"/>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C59" s="2"/>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C60" s="2"/>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C61" s="2"/>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.3">
+      <c r="C84" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1"/>
-    <hyperlink ref="G2"/>
+    <hyperlink ref="E2" display="https://accounts.google.com/o/oauth2/v2/auth?scope=https://www.googleapis.com/auth/userinfo.email&amp;auth_url=https://accounts.google.com/o/oauth2/v2/auth&amp;client_id=692183103107-p0m7ent2hk7suguv4vq22hjcfhcr43pj.apps.googleusercontent.com&amp;response_type=code&amp;r"/>
+    <hyperlink ref="E4" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating the cucumber bdd
</commit_message>
<xml_diff>
--- a/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
+++ b/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updating AddPlace test in MapsAPI -cucumber integration
</commit_message>
<xml_diff>
--- a/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
+++ b/RestAPI-Test-Framework/ExecutionFiles/Maps/Maps.xlsx
@@ -163,10 +163,10 @@
     <t>types</t>
   </si>
   <si>
-    <t>My Shop:Raymonds , The Stopper's Stop</t>
-  </si>
-  <si>
     <t>accuracy</t>
+  </si>
+  <si>
+    <t>Raymonds , The Stoppers</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -739,7 +739,7 @@
         <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="9">
         <v>50</v>
@@ -796,7 +796,7 @@
         <v>43</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>